<commit_message>
sort bar chart, add treemap data, styling,
</commit_message>
<xml_diff>
--- a/raw_data/Chart3/Number_of_Species_total_critical_threatened.xlsx
+++ b/raw_data/Chart3/Number_of_Species_total_critical_threatened.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karin.guedel@fhnw.ch/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karin.guedel@fhnw.ch/WebstormProjects/guedelkohler/raw_data/Chart3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC95988-5479-4A4E-91A3-80C0D7732F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7713D9E2-CBCC-B44C-BBA8-8743A661C3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1880" yWindow="960" windowWidth="26240" windowHeight="14340" activeTab="1" xr2:uid="{A72C8E66-A1BE-4243-9410-DC83B411B436}"/>
+    <workbookView xWindow="11160" yWindow="1540" windowWidth="12920" windowHeight="14340" xr2:uid="{A72C8E66-A1BE-4243-9410-DC83B411B436}"/>
   </bookViews>
   <sheets>
     <sheet name="Anzahl_Arten_CH" sheetId="1" r:id="rId1"/>
     <sheet name="SäugetiereCH" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="439">
   <si>
     <t>Switzerland</t>
   </si>
@@ -45,15 +45,6 @@
     <t>known species</t>
   </si>
   <si>
-    <t>critically engangered</t>
-  </si>
-  <si>
-    <t>engangered</t>
-  </si>
-  <si>
-    <t>vulnerable</t>
-  </si>
-  <si>
     <t>threatened</t>
   </si>
   <si>
@@ -1348,14 +1339,30 @@
   </si>
   <si>
     <t>NA = erratisch, allochton</t>
+  </si>
+  <si>
+    <t>nicht gefährdet</t>
+  </si>
+  <si>
+    <t>gefährdet Total</t>
+  </si>
+  <si>
+    <t>stark gefährdet</t>
+  </si>
+  <si>
+    <t>Vom Aussterben bedroht</t>
+  </si>
+  <si>
+    <t>verletzlich</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0_ ;\-#,##0.0\ "/>
+    <numFmt numFmtId="165" formatCode="#\'##0.0_ ;\-#\'##0.0\ "/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -1496,7 +1503,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1530,6 +1537,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1893,15 +1903,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02599600-F6DE-1A4E-85B3-4A539DE56100}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1909,21 +1919,27 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="G1" s="13" t="s">
+        <v>434</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="B2" s="5">
         <v>97</v>
@@ -1940,10 +1956,18 @@
       <c r="F2" s="5">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="14">
+        <f>B2-F2</f>
+        <v>64</v>
+      </c>
+      <c r="H2" s="15">
+        <f>SUM(C2:E2)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" s="5">
         <v>205</v>
@@ -1960,10 +1984,18 @@
       <c r="F3" s="5">
         <v>76</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="14">
+        <f t="shared" ref="G3:G12" si="0">B3-F3</f>
+        <v>129</v>
+      </c>
+      <c r="H3" s="15">
+        <f t="shared" ref="H3:H12" si="1">SUM(C3:E3)</f>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4" s="5">
         <v>19</v>
@@ -1980,10 +2012,18 @@
       <c r="F4" s="5">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="14">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H4" s="15">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B5" s="5">
         <v>19</v>
@@ -2000,10 +2040,18 @@
       <c r="F5" s="5">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="14">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H5" s="15">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6" s="5">
         <v>90</v>
@@ -2020,30 +2068,46 @@
       <c r="F6" s="5">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="28" x14ac:dyDescent="0.2">
+      <c r="G6" s="14">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="H6" s="15">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="28" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="28" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="G7" s="14" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H7" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="28" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B8" s="5">
         <v>90</v>
@@ -2060,10 +2124,18 @@
       <c r="F8" s="5">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="28" x14ac:dyDescent="0.2">
+      <c r="G8" s="14">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="H8" s="15">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B9" s="5">
         <v>2866</v>
@@ -2080,10 +2152,18 @@
       <c r="F9" s="5">
         <v>780</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" s="14">
+        <f t="shared" si="0"/>
+        <v>2086</v>
+      </c>
+      <c r="H9" s="15">
+        <f t="shared" si="1"/>
+        <v>670</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B10" s="5">
         <v>1153</v>
@@ -2100,10 +2180,18 @@
       <c r="F10" s="5">
         <v>387</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="14">
+        <f t="shared" si="0"/>
+        <v>766</v>
+      </c>
+      <c r="H10" s="15">
+        <f t="shared" si="1"/>
+        <v>387</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B11" s="5">
         <v>786</v>
@@ -2120,10 +2208,18 @@
       <c r="F11" s="5">
         <v>257</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="28" x14ac:dyDescent="0.2">
+      <c r="G11" s="14">
+        <f t="shared" si="0"/>
+        <v>529</v>
+      </c>
+      <c r="H11" s="15">
+        <f t="shared" si="1"/>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="28" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B12" s="5">
         <v>3118</v>
@@ -2140,23 +2236,31 @@
       <c r="F12" s="5">
         <v>1075</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" s="14">
+        <f t="shared" si="0"/>
+        <v>2043</v>
+      </c>
+      <c r="H12" s="15">
+        <f t="shared" si="1"/>
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="8">
         <f>SUM(B3:B12)</f>
         <v>8346</v>
       </c>
       <c r="C13" s="8">
-        <f t="shared" ref="C13:E13" si="0">SUM(C3:C12)</f>
+        <f t="shared" ref="C13:E13" si="2">SUM(C3:C12)</f>
         <v>548</v>
       </c>
       <c r="D13" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>809</v>
       </c>
       <c r="E13" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1203</v>
       </c>
       <c r="F13" s="8">
@@ -2172,7 +2276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C182423-B18D-E844-9755-412790554417}">
   <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
@@ -2180,2181 +2284,2181 @@
   <sheetData>
     <row r="1" spans="1:10" ht="28" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="F1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="E2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="F2" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="G2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="H2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="I2" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="J2" s="11" t="s">
         <v>34</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="F3" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="G3" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="H3" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="I3" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>45</v>
-      </c>
       <c r="J3" s="11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C4" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="G4" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="H4" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="I4" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="J4" s="11" t="s">
         <v>50</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="F5" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="G5" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="H5" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="I5" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="G5" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>61</v>
-      </c>
       <c r="J5" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C6" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="G6" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="H6" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="I6" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="G6" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>68</v>
-      </c>
       <c r="J6" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E7" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="I7" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="G7" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>73</v>
-      </c>
       <c r="J7" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D8" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="H8" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="I8" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="G8" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>79</v>
-      </c>
       <c r="J8" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B9" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="F9" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="G9" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="H9" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="I9" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="G9" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>87</v>
-      </c>
       <c r="J9" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D10" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="H10" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="I10" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G10" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>93</v>
-      </c>
       <c r="J10" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D11" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="G11" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="H11" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="I11" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="J11" s="11" t="s">
         <v>97</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E12" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H12" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="I12" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="G12" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>105</v>
-      </c>
       <c r="J12" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E13" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="H13" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="I13" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="G13" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>110</v>
-      </c>
       <c r="J13" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D14" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="G14" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="H14" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="I14" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="G14" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>116</v>
-      </c>
       <c r="J14" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B15" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="E15" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="F15" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="G15" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="H15" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="I15" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="G15" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>124</v>
-      </c>
       <c r="J15" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C16" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F16" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="G16" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="H16" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="I16" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="G16" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>131</v>
-      </c>
       <c r="J16" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C17" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="F17" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="G17" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="H17" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="I17" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="G17" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>138</v>
-      </c>
       <c r="J17" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D18" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="G18" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="H18" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="I18" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="G18" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>144</v>
-      </c>
       <c r="J18" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D19" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="G19" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="H19" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="I19" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="G19" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>150</v>
-      </c>
       <c r="J19" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D20" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="G20" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="H20" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="I20" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="G20" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>156</v>
-      </c>
       <c r="J20" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D21" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="G21" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="H21" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="I21" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="G21" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>162</v>
-      </c>
       <c r="J21" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C22" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="F22" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="G22" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="H22" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="I22" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="G22" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="I22" s="11" t="s">
-        <v>169</v>
-      </c>
       <c r="J22" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="M22" s="11" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D23" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="G23" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="H23" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="I23" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="G23" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="H23" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="I23" s="11" t="s">
-        <v>175</v>
-      </c>
       <c r="J23" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C24" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="F24" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="G24" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="H24" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="I24" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="G24" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="I24" s="11" t="s">
-        <v>182</v>
-      </c>
       <c r="J24" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D25" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="G25" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="H25" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="F25" s="12" t="s">
+      <c r="I25" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="G25" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="I25" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="J25" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E26" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="H26" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="I26" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="G26" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="H26" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="I26" s="11" t="s">
-        <v>193</v>
-      </c>
       <c r="J26" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D27" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="G27" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="H27" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="I27" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="G27" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="I27" s="11" t="s">
-        <v>199</v>
-      </c>
       <c r="J27" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E28" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="H28" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="F28" s="12" t="s">
+      <c r="I28" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="G28" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="H28" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="I28" s="11" t="s">
-        <v>204</v>
-      </c>
       <c r="J28" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E29" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="H29" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="F29" s="12" t="s">
+      <c r="I29" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="G29" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="H29" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="I29" s="11" t="s">
-        <v>209</v>
-      </c>
       <c r="J29" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E30" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="H30" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="F30" s="12" t="s">
+      <c r="I30" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="G30" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="H30" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="I30" s="11" t="s">
-        <v>214</v>
-      </c>
       <c r="J30" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D31" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="G31" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="H31" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="F31" s="12" t="s">
+      <c r="I31" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="G31" s="11" t="s">
-        <v>218</v>
-      </c>
-      <c r="H31" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="I31" s="11" t="s">
-        <v>220</v>
-      </c>
       <c r="J31" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D32" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="G32" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="H32" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="F32" s="12" t="s">
+      <c r="I32" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="G32" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="H32" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I32" s="11" t="s">
-        <v>226</v>
-      </c>
       <c r="J32" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D33" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="G33" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="H33" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F33" s="12" t="s">
+      <c r="I33" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="G33" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="H33" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="I33" s="11" t="s">
-        <v>232</v>
-      </c>
       <c r="J33" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D34" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="G34" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="E34" s="11" t="s">
+      <c r="H34" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="F34" s="12" t="s">
+      <c r="I34" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="G34" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="H34" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="I34" s="11" t="s">
-        <v>238</v>
-      </c>
       <c r="J34" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D35" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="G35" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="H35" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="F35" s="12" t="s">
+      <c r="I35" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="G35" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="H35" s="11" t="s">
-        <v>243</v>
-      </c>
-      <c r="I35" s="11" t="s">
-        <v>244</v>
-      </c>
       <c r="J35" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E36" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="H36" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="F36" s="12" t="s">
+      <c r="I36" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="G36" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="H36" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="I36" s="11" t="s">
-        <v>249</v>
-      </c>
       <c r="J36" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E37" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="H37" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="F37" s="12" t="s">
+      <c r="I37" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="G37" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="H37" s="11" t="s">
-        <v>253</v>
-      </c>
-      <c r="I37" s="11" t="s">
-        <v>254</v>
-      </c>
       <c r="J37" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E38" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="H38" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="F38" s="12" t="s">
+      <c r="I38" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="G38" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="H38" s="11" t="s">
-        <v>258</v>
-      </c>
-      <c r="I38" s="11" t="s">
-        <v>259</v>
-      </c>
       <c r="J38" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F39" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="I39" s="11" t="s">
         <v>260</v>
       </c>
-      <c r="G39" s="11" t="s">
-        <v>261</v>
-      </c>
-      <c r="H39" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="I39" s="11" t="s">
-        <v>263</v>
-      </c>
       <c r="J39" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C40" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="F40" s="12" t="s">
         <v>264</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="G40" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="E40" s="11" t="s">
+      <c r="H40" s="11" t="s">
         <v>266</v>
       </c>
-      <c r="F40" s="12" t="s">
+      <c r="I40" s="11" t="s">
         <v>267</v>
       </c>
-      <c r="G40" s="11" t="s">
-        <v>268</v>
-      </c>
-      <c r="H40" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="I40" s="11" t="s">
-        <v>270</v>
-      </c>
       <c r="J40" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C41" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="F41" s="12" t="s">
         <v>271</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="G41" s="11" t="s">
         <v>272</v>
       </c>
-      <c r="E41" s="11" t="s">
+      <c r="H41" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="F41" s="12" t="s">
+      <c r="I41" s="11" t="s">
         <v>274</v>
       </c>
-      <c r="G41" s="11" t="s">
-        <v>275</v>
-      </c>
-      <c r="H41" s="11" t="s">
-        <v>276</v>
-      </c>
-      <c r="I41" s="11" t="s">
-        <v>277</v>
-      </c>
       <c r="J41" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C42" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="F42" s="12" t="s">
         <v>278</v>
       </c>
-      <c r="D42" s="11" t="s">
+      <c r="G42" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="E42" s="11" t="s">
+      <c r="H42" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="F42" s="12" t="s">
+      <c r="I42" s="11" t="s">
         <v>281</v>
       </c>
-      <c r="G42" s="11" t="s">
-        <v>282</v>
-      </c>
-      <c r="H42" s="11" t="s">
-        <v>283</v>
-      </c>
-      <c r="I42" s="11" t="s">
-        <v>284</v>
-      </c>
       <c r="J42" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D43" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="F43" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="G43" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="E43" s="11" t="s">
+      <c r="H43" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="F43" s="12" t="s">
+      <c r="I43" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="G43" s="11" t="s">
+      <c r="J43" s="11" t="s">
         <v>288</v>
-      </c>
-      <c r="H43" s="11" t="s">
-        <v>289</v>
-      </c>
-      <c r="I43" s="11" t="s">
-        <v>290</v>
-      </c>
-      <c r="J43" s="11" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E44" s="11" t="s">
+        <v>289</v>
+      </c>
+      <c r="F44" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="G44" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="H44" s="11" t="s">
         <v>292</v>
       </c>
-      <c r="F44" s="12" t="s">
+      <c r="I44" s="11" t="s">
         <v>293</v>
       </c>
-      <c r="G44" s="11" t="s">
-        <v>294</v>
-      </c>
-      <c r="H44" s="11" t="s">
-        <v>295</v>
-      </c>
-      <c r="I44" s="11" t="s">
-        <v>296</v>
-      </c>
       <c r="J44" s="11" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D45" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="G45" s="11" t="s">
         <v>297</v>
       </c>
-      <c r="E45" s="11" t="s">
+      <c r="H45" s="11" t="s">
         <v>298</v>
       </c>
-      <c r="F45" s="12" t="s">
+      <c r="I45" s="11" t="s">
         <v>299</v>
       </c>
-      <c r="G45" s="11" t="s">
-        <v>300</v>
-      </c>
-      <c r="H45" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="I45" s="11" t="s">
-        <v>302</v>
-      </c>
       <c r="J45" s="11" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C46" s="11" t="s">
+        <v>300</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>302</v>
+      </c>
+      <c r="F46" s="12" t="s">
         <v>303</v>
       </c>
-      <c r="D46" s="11" t="s">
+      <c r="G46" s="11" t="s">
         <v>304</v>
       </c>
-      <c r="E46" s="11" t="s">
+      <c r="H46" s="11" t="s">
         <v>305</v>
       </c>
-      <c r="F46" s="12" t="s">
+      <c r="I46" s="11" t="s">
         <v>306</v>
       </c>
-      <c r="G46" s="11" t="s">
-        <v>307</v>
-      </c>
-      <c r="H46" s="11" t="s">
-        <v>308</v>
-      </c>
-      <c r="I46" s="11" t="s">
-        <v>309</v>
-      </c>
       <c r="J46" s="11" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C47" s="11" t="s">
+        <v>307</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="F47" s="12" t="s">
         <v>310</v>
       </c>
-      <c r="D47" s="11" t="s">
+      <c r="G47" s="11" t="s">
         <v>311</v>
       </c>
-      <c r="E47" s="11" t="s">
+      <c r="H47" s="11" t="s">
         <v>312</v>
       </c>
-      <c r="F47" s="12" t="s">
-        <v>313</v>
-      </c>
-      <c r="G47" s="11" t="s">
-        <v>314</v>
-      </c>
-      <c r="H47" s="11" t="s">
-        <v>315</v>
-      </c>
       <c r="I47" s="11" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="J47" s="11" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D48" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="G48" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="E48" s="11" t="s">
+      <c r="H48" s="11" t="s">
         <v>317</v>
       </c>
-      <c r="F48" s="12" t="s">
+      <c r="I48" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="G48" s="11" t="s">
-        <v>319</v>
-      </c>
-      <c r="H48" s="11" t="s">
-        <v>320</v>
-      </c>
-      <c r="I48" s="11" t="s">
-        <v>321</v>
-      </c>
       <c r="J48" s="11" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D49" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>320</v>
+      </c>
+      <c r="F49" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="G49" s="11" t="s">
         <v>322</v>
       </c>
-      <c r="E49" s="11" t="s">
+      <c r="H49" s="11" t="s">
         <v>323</v>
       </c>
-      <c r="F49" s="12" t="s">
-        <v>324</v>
-      </c>
-      <c r="G49" s="11" t="s">
-        <v>325</v>
-      </c>
-      <c r="H49" s="11" t="s">
-        <v>326</v>
-      </c>
       <c r="I49" s="11" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="J49" s="11" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D50" s="11" t="s">
+        <v>324</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="G50" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="E50" s="11" t="s">
+      <c r="H50" s="11" t="s">
         <v>328</v>
       </c>
-      <c r="F50" s="12" t="s">
+      <c r="I50" s="11" t="s">
         <v>329</v>
       </c>
-      <c r="G50" s="11" t="s">
-        <v>330</v>
-      </c>
-      <c r="H50" s="11" t="s">
-        <v>331</v>
-      </c>
-      <c r="I50" s="11" t="s">
-        <v>332</v>
-      </c>
       <c r="J50" s="11" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C51" s="11" t="s">
+        <v>330</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>331</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>332</v>
+      </c>
+      <c r="F51" s="12" t="s">
         <v>333</v>
       </c>
-      <c r="D51" s="11" t="s">
+      <c r="G51" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="E51" s="11" t="s">
+      <c r="H51" s="11" t="s">
         <v>335</v>
       </c>
-      <c r="F51" s="12" t="s">
+      <c r="I51" s="11" t="s">
         <v>336</v>
       </c>
-      <c r="G51" s="11" t="s">
-        <v>337</v>
-      </c>
-      <c r="H51" s="11" t="s">
-        <v>338</v>
-      </c>
-      <c r="I51" s="11" t="s">
-        <v>339</v>
-      </c>
       <c r="J51" s="11" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E52" s="11" t="s">
+        <v>337</v>
+      </c>
+      <c r="F52" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="G52" s="11" t="s">
+        <v>339</v>
+      </c>
+      <c r="H52" s="11" t="s">
         <v>340</v>
       </c>
-      <c r="F52" s="12" t="s">
+      <c r="I52" s="11" t="s">
         <v>341</v>
       </c>
-      <c r="G52" s="11" t="s">
-        <v>342</v>
-      </c>
-      <c r="H52" s="11" t="s">
-        <v>343</v>
-      </c>
-      <c r="I52" s="11" t="s">
-        <v>344</v>
-      </c>
       <c r="J52" s="11" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D53" s="11" t="s">
+        <v>342</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>343</v>
+      </c>
+      <c r="F53" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="G53" s="11" t="s">
         <v>345</v>
       </c>
-      <c r="E53" s="11" t="s">
+      <c r="H53" s="11" t="s">
         <v>346</v>
       </c>
-      <c r="F53" s="12" t="s">
+      <c r="I53" s="11" t="s">
         <v>347</v>
       </c>
-      <c r="G53" s="11" t="s">
-        <v>348</v>
-      </c>
-      <c r="H53" s="11" t="s">
-        <v>349</v>
-      </c>
-      <c r="I53" s="11" t="s">
-        <v>350</v>
-      </c>
       <c r="J53" s="11" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D54" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="E54" s="11" t="s">
+        <v>349</v>
+      </c>
+      <c r="F54" s="12" t="s">
+        <v>350</v>
+      </c>
+      <c r="G54" s="11" t="s">
         <v>351</v>
       </c>
-      <c r="E54" s="11" t="s">
+      <c r="H54" s="11" t="s">
         <v>352</v>
       </c>
-      <c r="F54" s="12" t="s">
+      <c r="I54" s="11" t="s">
         <v>353</v>
       </c>
-      <c r="G54" s="11" t="s">
-        <v>354</v>
-      </c>
-      <c r="H54" s="11" t="s">
-        <v>355</v>
-      </c>
-      <c r="I54" s="11" t="s">
-        <v>356</v>
-      </c>
       <c r="J54" s="11" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C55" s="11" t="s">
+        <v>354</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>355</v>
+      </c>
+      <c r="E55" s="11" t="s">
+        <v>356</v>
+      </c>
+      <c r="F55" s="12" t="s">
         <v>357</v>
       </c>
-      <c r="D55" s="11" t="s">
+      <c r="G55" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="E55" s="11" t="s">
+      <c r="H55" s="11" t="s">
         <v>359</v>
       </c>
-      <c r="F55" s="12" t="s">
+      <c r="I55" s="11" t="s">
         <v>360</v>
       </c>
-      <c r="G55" s="11" t="s">
+      <c r="J55" s="11" t="s">
         <v>361</v>
-      </c>
-      <c r="H55" s="11" t="s">
-        <v>362</v>
-      </c>
-      <c r="I55" s="11" t="s">
-        <v>363</v>
-      </c>
-      <c r="J55" s="11" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D56" s="11" t="s">
+        <v>362</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>363</v>
+      </c>
+      <c r="F56" s="12" t="s">
+        <v>364</v>
+      </c>
+      <c r="G56" s="11" t="s">
         <v>365</v>
       </c>
-      <c r="E56" s="11" t="s">
+      <c r="H56" s="11" t="s">
         <v>366</v>
       </c>
-      <c r="F56" s="12" t="s">
+      <c r="I56" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="G56" s="11" t="s">
-        <v>368</v>
-      </c>
-      <c r="H56" s="11" t="s">
-        <v>369</v>
-      </c>
-      <c r="I56" s="11" t="s">
-        <v>370</v>
-      </c>
       <c r="J56" s="11" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D57" s="11" t="s">
+        <v>368</v>
+      </c>
+      <c r="E57" s="11" t="s">
+        <v>369</v>
+      </c>
+      <c r="F57" s="12" t="s">
+        <v>370</v>
+      </c>
+      <c r="G57" s="11" t="s">
         <v>371</v>
       </c>
-      <c r="E57" s="11" t="s">
+      <c r="H57" s="11" t="s">
         <v>372</v>
       </c>
-      <c r="F57" s="12" t="s">
+      <c r="I57" s="11" t="s">
         <v>373</v>
       </c>
-      <c r="G57" s="11" t="s">
-        <v>374</v>
-      </c>
-      <c r="H57" s="11" t="s">
-        <v>375</v>
-      </c>
-      <c r="I57" s="11" t="s">
-        <v>376</v>
-      </c>
       <c r="J57" s="11" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="E58" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="F58" s="12" t="s">
+        <v>375</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>376</v>
+      </c>
+      <c r="H58" s="11" t="s">
         <v>377</v>
       </c>
-      <c r="F58" s="12" t="s">
+      <c r="I58" s="11" t="s">
         <v>378</v>
       </c>
-      <c r="G58" s="11" t="s">
-        <v>379</v>
-      </c>
-      <c r="H58" s="11" t="s">
-        <v>380</v>
-      </c>
-      <c r="I58" s="11" t="s">
-        <v>381</v>
-      </c>
       <c r="J58" s="11" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C59" s="11" t="s">
+        <v>379</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="E59" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="F59" s="12" t="s">
         <v>382</v>
       </c>
-      <c r="D59" s="11" t="s">
+      <c r="G59" s="11" t="s">
         <v>383</v>
       </c>
-      <c r="E59" s="11" t="s">
+      <c r="H59" s="11" t="s">
         <v>384</v>
       </c>
-      <c r="F59" s="12" t="s">
+      <c r="I59" s="11" t="s">
         <v>385</v>
       </c>
-      <c r="G59" s="11" t="s">
+      <c r="J59" s="11" t="s">
         <v>386</v>
-      </c>
-      <c r="H59" s="11" t="s">
-        <v>387</v>
-      </c>
-      <c r="I59" s="11" t="s">
-        <v>388</v>
-      </c>
-      <c r="J59" s="11" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E60" s="11" t="s">
+        <v>387</v>
+      </c>
+      <c r="F60" s="12" t="s">
+        <v>388</v>
+      </c>
+      <c r="G60" s="11" t="s">
+        <v>389</v>
+      </c>
+      <c r="H60" s="11" t="s">
         <v>390</v>
       </c>
-      <c r="F60" s="12" t="s">
+      <c r="I60" s="11" t="s">
         <v>391</v>
       </c>
-      <c r="G60" s="11" t="s">
+      <c r="J60" s="11" t="s">
         <v>392</v>
-      </c>
-      <c r="H60" s="11" t="s">
-        <v>393</v>
-      </c>
-      <c r="I60" s="11" t="s">
-        <v>394</v>
-      </c>
-      <c r="J60" s="11" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E61" s="11" t="s">
+        <v>393</v>
+      </c>
+      <c r="F61" s="12" t="s">
+        <v>394</v>
+      </c>
+      <c r="G61" s="11" t="s">
+        <v>395</v>
+      </c>
+      <c r="H61" s="11" t="s">
         <v>396</v>
       </c>
-      <c r="F61" s="12" t="s">
+      <c r="I61" s="11" t="s">
         <v>397</v>
       </c>
-      <c r="G61" s="11" t="s">
-        <v>398</v>
-      </c>
-      <c r="H61" s="11" t="s">
-        <v>399</v>
-      </c>
-      <c r="I61" s="11" t="s">
-        <v>400</v>
-      </c>
       <c r="J61" s="11" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E62" s="11" t="s">
+        <v>398</v>
+      </c>
+      <c r="F62" s="12" t="s">
+        <v>399</v>
+      </c>
+      <c r="G62" s="11" t="s">
+        <v>400</v>
+      </c>
+      <c r="H62" s="11" t="s">
         <v>401</v>
       </c>
-      <c r="F62" s="12" t="s">
+      <c r="I62" s="11" t="s">
         <v>402</v>
       </c>
-      <c r="G62" s="11" t="s">
-        <v>403</v>
-      </c>
-      <c r="H62" s="11" t="s">
-        <v>404</v>
-      </c>
-      <c r="I62" s="11" t="s">
-        <v>405</v>
-      </c>
       <c r="J62" s="11" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D63" s="11" t="s">
+        <v>403</v>
+      </c>
+      <c r="E63" s="11" t="s">
+        <v>404</v>
+      </c>
+      <c r="F63" s="12" t="s">
+        <v>405</v>
+      </c>
+      <c r="G63" s="11" t="s">
         <v>406</v>
       </c>
-      <c r="E63" s="11" t="s">
+      <c r="H63" s="11" t="s">
         <v>407</v>
       </c>
-      <c r="F63" s="12" t="s">
+      <c r="I63" s="11" t="s">
         <v>408</v>
       </c>
-      <c r="G63" s="11" t="s">
-        <v>409</v>
-      </c>
-      <c r="H63" s="11" t="s">
-        <v>410</v>
-      </c>
-      <c r="I63" s="11" t="s">
-        <v>411</v>
-      </c>
       <c r="J63" s="11" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F64" s="12" t="s">
+        <v>409</v>
+      </c>
+      <c r="G64" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="H64" s="11" t="s">
+        <v>411</v>
+      </c>
+      <c r="I64" s="11" t="s">
         <v>412</v>
       </c>
-      <c r="G64" s="11" t="s">
-        <v>413</v>
-      </c>
-      <c r="H64" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="I64" s="11" t="s">
-        <v>415</v>
-      </c>
       <c r="J64" s="11" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D65" s="11" t="s">
+        <v>413</v>
+      </c>
+      <c r="E65" s="11" t="s">
+        <v>414</v>
+      </c>
+      <c r="F65" s="12" t="s">
+        <v>415</v>
+      </c>
+      <c r="G65" s="11" t="s">
         <v>416</v>
       </c>
-      <c r="E65" s="11" t="s">
+      <c r="H65" s="11" t="s">
         <v>417</v>
       </c>
-      <c r="F65" s="12" t="s">
+      <c r="I65" s="11" t="s">
         <v>418</v>
       </c>
-      <c r="G65" s="11" t="s">
-        <v>419</v>
-      </c>
-      <c r="H65" s="11" t="s">
-        <v>420</v>
-      </c>
-      <c r="I65" s="11" t="s">
-        <v>421</v>
-      </c>
       <c r="J65" s="11" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F66" s="12" t="s">
+        <v>419</v>
+      </c>
+      <c r="G66" s="11" t="s">
+        <v>420</v>
+      </c>
+      <c r="H66" s="11" t="s">
+        <v>421</v>
+      </c>
+      <c r="I66" s="11" t="s">
         <v>422</v>
       </c>
-      <c r="G66" s="11" t="s">
-        <v>423</v>
-      </c>
-      <c r="H66" s="11" t="s">
-        <v>424</v>
-      </c>
-      <c r="I66" s="11" t="s">
-        <v>425</v>
-      </c>
       <c r="J66" s="11" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E67" s="11" t="s">
+        <v>423</v>
+      </c>
+      <c r="F67" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="G67" s="11" t="s">
+        <v>425</v>
+      </c>
+      <c r="H67" s="11" t="s">
         <v>426</v>
       </c>
-      <c r="F67" s="12" t="s">
+      <c r="I67" s="11" t="s">
         <v>427</v>
       </c>
-      <c r="G67" s="11" t="s">
-        <v>428</v>
-      </c>
-      <c r="H67" s="11" t="s">
-        <v>429</v>
-      </c>
-      <c r="I67" s="11" t="s">
-        <v>430</v>
-      </c>
       <c r="J67" s="11" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E68" s="11" t="s">
+        <v>428</v>
+      </c>
+      <c r="F68" s="12" t="s">
+        <v>429</v>
+      </c>
+      <c r="G68" s="11" t="s">
+        <v>430</v>
+      </c>
+      <c r="H68" s="11" t="s">
         <v>431</v>
       </c>
-      <c r="F68" s="12" t="s">
+      <c r="I68" s="11" t="s">
         <v>432</v>
       </c>
-      <c r="G68" s="11" t="s">
-        <v>433</v>
-      </c>
-      <c r="H68" s="11" t="s">
-        <v>434</v>
-      </c>
-      <c r="I68" s="11" t="s">
-        <v>435</v>
-      </c>
       <c r="J68" s="11" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
optimizing treemap, tests with interactive treemaps, icons, styling, colors
</commit_message>
<xml_diff>
--- a/raw_data/Chart3/Number_of_Species_total_critical_threatened.xlsx
+++ b/raw_data/Chart3/Number_of_Species_total_critical_threatened.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karin.guedel@fhnw.ch/WebstormProjects/guedelkohler/raw_data/Chart3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7713D9E2-CBCC-B44C-BBA8-8743A661C3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2D946A-F00C-0747-B395-739A3A78245E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11160" yWindow="1540" windowWidth="12920" windowHeight="14340" xr2:uid="{A72C8E66-A1BE-4243-9410-DC83B411B436}"/>
+    <workbookView xWindow="15540" yWindow="500" windowWidth="13060" windowHeight="16480" xr2:uid="{A72C8E66-A1BE-4243-9410-DC83B411B436}"/>
   </bookViews>
   <sheets>
     <sheet name="Anzahl_Arten_CH" sheetId="1" r:id="rId1"/>
@@ -1503,7 +1503,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1537,7 +1537,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -1906,10 +1905,13 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="20.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1930,10 +1932,10 @@
       <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="3" t="s">
         <v>434</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="3" t="s">
         <v>435</v>
       </c>
     </row>
@@ -1956,11 +1958,11 @@
       <c r="F2" s="5">
         <v>33</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="13">
         <f>B2-F2</f>
         <v>64</v>
       </c>
-      <c r="H2" s="15">
+      <c r="H2" s="14">
         <f>SUM(C2:E2)</f>
         <v>33</v>
       </c>
@@ -1984,11 +1986,11 @@
       <c r="F3" s="5">
         <v>76</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="13">
         <f t="shared" ref="G3:G12" si="0">B3-F3</f>
         <v>129</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="14">
         <f t="shared" ref="H3:H12" si="1">SUM(C3:E3)</f>
         <v>76</v>
       </c>
@@ -2012,11 +2014,11 @@
       <c r="F4" s="5">
         <v>13</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="13">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="14">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
@@ -2040,11 +2042,11 @@
       <c r="F5" s="5">
         <v>14</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="13">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="14">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
@@ -2068,11 +2070,11 @@
       <c r="F6" s="5">
         <v>34</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="13">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="14">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
@@ -2096,11 +2098,11 @@
       <c r="F7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="14" t="e">
+      <c r="G7" s="13" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2124,11 +2126,11 @@
       <c r="F8" s="5">
         <v>34</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="14">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
@@ -2152,11 +2154,11 @@
       <c r="F9" s="5">
         <v>780</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2086</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="14">
         <f t="shared" si="1"/>
         <v>670</v>
       </c>
@@ -2180,11 +2182,11 @@
       <c r="F10" s="5">
         <v>387</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>766</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="14">
         <f t="shared" si="1"/>
         <v>387</v>
       </c>
@@ -2208,11 +2210,11 @@
       <c r="F11" s="5">
         <v>257</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>529</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="14">
         <f t="shared" si="1"/>
         <v>257</v>
       </c>
@@ -2236,11 +2238,11 @@
       <c r="F12" s="5">
         <v>1075</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="13">
         <f t="shared" si="0"/>
         <v>2043</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H12" s="14">
         <f t="shared" si="1"/>
         <v>1075</v>
       </c>

</xml_diff>